<commit_message>
June 7 WMP update
</commit_message>
<xml_diff>
--- a/WMP25/SDGE Response MGRA-SDGE-2025WMP-03_Q2_Revised 4.19.24-TUGCustomers-jwm.xlsx
+++ b/WMP25/SDGE Response MGRA-SDGE-2025WMP-03_Q2_Revised 4.19.24-TUGCustomers-jwm.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD74EB1E-B51A-D041-BB4C-908998761B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BC9221F-8733-2841-B128-E439E42C1DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="-19540" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="11" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="92">
   <si>
     <t>a) Order Number</t>
   </si>
@@ -306,6 +328,15 @@
   </si>
   <si>
     <t>PSPS Circuit Minutes</t>
+  </si>
+  <si>
+    <t>Log cpcm</t>
+  </si>
+  <si>
+    <t>Bins</t>
+  </si>
+  <si>
+    <t>Binned cost</t>
   </si>
 </sst>
 </file>
@@ -314,7 +345,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -393,7 +424,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -406,12 +437,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -428,7 +458,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -487,6 +517,1074 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SDGE 2025</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LOG10</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Cost $/min </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Averted PSPS per Customer-Circuit Segment</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Final!$Q$5:$Q$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Final!$R$5:$R$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3366-7C4E-9BF6-055D7D9DC3E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="882685408"/>
+        <c:axId val="882687120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="882685408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Log10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> $</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="882687120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="882687120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Circuit</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Segments</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="882685408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4572BF3-7596-0888-9A43-1ADD64485A0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1006,7 +2104,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00E8E3C7-0BB8-2B40-AC89-FCD73939A792}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Circuit Segment">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00E8E3C7-0BB8-2B40-AC89-FCD73939A792}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Circuit Segment">
   <location ref="A3:E17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -1232,7 +2330,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B593503-77B0-6847-9B16-10958CAFD6D6}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B593503-77B0-6847-9B16-10958CAFD6D6}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -2787,10 +3885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61046B4B-B355-C744-BCA0-3F46871DE0A6}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2803,13 +3901,13 @@
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="18" style="11" customWidth="1"/>
+    <col min="10" max="10" width="18" style="10" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2817,71 +3915,80 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:14" s="16" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+    <row r="2" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:18" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="16" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="O3" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4">
         <v>213</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4">
         <v>0.5</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4">
         <v>3338</v>
       </c>
       <c r="F4">
         <v>0.5</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <f>3000000*F4</f>
         <v>1500000</v>
       </c>
@@ -2891,15 +3998,15 @@
       <c r="I4">
         <v>3338</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="10">
         <f>G4/H4</f>
         <v>7042.2535211267605</v>
       </c>
-      <c r="K4" s="12" t="str">
+      <c r="K4" s="11" t="str">
         <f>IF(J4&gt;60000,"Y","")</f>
         <v/>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <f>IF(K4="Y",60000*H4,G4)</f>
         <v>1500000</v>
       </c>
@@ -2907,31 +4014,39 @@
         <f>H4*I4</f>
         <v>710994</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="14">
         <f>G4/M4</f>
         <v>2.109722444915147</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="O4">
+        <f>LOG(N4)</f>
+        <v>0.32422532327371562</v>
+      </c>
+      <c r="R4" cm="1">
+        <f t="array" ref="R4:R15">FREQUENCY(O4:O17,Q5:Q15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5">
         <v>190</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5">
         <v>6.3000000000000007</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5">
         <v>3338</v>
       </c>
       <c r="F5">
         <v>6.3000000000000007</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <f t="shared" ref="G5:G17" si="0">3000000*F5</f>
         <v>18900000.000000004</v>
       </c>
@@ -2941,15 +4056,15 @@
       <c r="I5">
         <v>3338</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="10">
         <f t="shared" ref="J5:J17" si="1">G5/H5</f>
         <v>99473.684210526335</v>
       </c>
-      <c r="K5" s="12" t="str">
+      <c r="K5" s="11" t="str">
         <f t="shared" ref="K5:K17" si="2">IF(J5&gt;60000,"Y","")</f>
         <v>Y</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <f t="shared" ref="L5:L16" si="3">IF(K5="Y",60000*H5,G5)</f>
         <v>11400000</v>
       </c>
@@ -2957,31 +4072,41 @@
         <f t="shared" ref="M5:M16" si="4">H5*I5</f>
         <v>634220</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="14">
         <f t="shared" ref="N5:N17" si="5">G5/M5</f>
         <v>29.800384724543541</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="O5">
+        <f t="shared" ref="O5:O17" si="6">LOG(N5)</f>
+        <v>1.4742218708771875</v>
+      </c>
+      <c r="Q5">
+        <v>-1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6">
         <v>78</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6">
         <v>7</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6">
         <v>13132</v>
       </c>
       <c r="F6">
         <v>7</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f t="shared" si="0"/>
         <v>21000000</v>
       </c>
@@ -2991,15 +4116,15 @@
       <c r="I6">
         <v>13132</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <f t="shared" si="1"/>
         <v>269230.76923076925</v>
       </c>
-      <c r="K6" s="12" t="str">
+      <c r="K6" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Y</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <f t="shared" si="3"/>
         <v>4680000</v>
       </c>
@@ -3007,31 +4132,42 @@
         <f t="shared" si="4"/>
         <v>1024296</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="14">
         <f t="shared" si="5"/>
         <v>20.501886173527964</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="O6">
+        <f t="shared" si="6"/>
+        <v>1.3117938179861364</v>
+      </c>
+      <c r="Q6">
+        <f>Q5+0.25</f>
+        <v>-0.75</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7">
         <v>261</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7">
         <v>2.04</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>20222</v>
       </c>
       <c r="F7">
         <v>2.04</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <f t="shared" si="0"/>
         <v>6120000</v>
       </c>
@@ -3041,15 +4177,15 @@
       <c r="I7">
         <v>20222</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <f t="shared" si="1"/>
         <v>23448.275862068964</v>
       </c>
-      <c r="K7" s="12" t="str">
+      <c r="K7" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <f t="shared" si="3"/>
         <v>6120000</v>
       </c>
@@ -3057,31 +4193,42 @@
         <f t="shared" si="4"/>
         <v>5277942</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="14">
         <f t="shared" si="5"/>
         <v>1.1595428672766772</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="O7">
+        <f t="shared" si="6"/>
+        <v>6.4286808754586977E-2</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ref="Q7:Q15" si="7">Q6+0.25</f>
+        <v>-0.5</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8">
         <v>132</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8">
         <v>10.719999999999999</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8">
         <v>20222</v>
       </c>
       <c r="F8">
         <v>10.719999999999999</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <f t="shared" si="0"/>
         <v>32159999.999999996</v>
       </c>
@@ -3091,15 +4238,15 @@
       <c r="I8">
         <v>20222</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <f t="shared" si="1"/>
         <v>243636.36363636362</v>
       </c>
-      <c r="K8" s="12" t="str">
+      <c r="K8" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Y</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <f t="shared" si="3"/>
         <v>7920000</v>
       </c>
@@ -3107,31 +4254,42 @@
         <f t="shared" si="4"/>
         <v>2669304</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="14">
         <f t="shared" si="5"/>
         <v>12.048084444484404</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="O8">
+        <f t="shared" si="6"/>
+        <v>1.0809180028178704</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="7"/>
+        <v>-0.25</v>
+      </c>
+      <c r="R8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>915</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9">
         <v>5</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>23206</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <f t="shared" si="0"/>
         <v>15000000</v>
       </c>
@@ -3141,15 +4299,15 @@
       <c r="I9">
         <v>23206</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <f t="shared" si="1"/>
         <v>16393.442622950821</v>
       </c>
-      <c r="K9" s="12" t="str">
+      <c r="K9" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <f t="shared" si="3"/>
         <v>15000000</v>
       </c>
@@ -3157,31 +4315,42 @@
         <f t="shared" si="4"/>
         <v>21233490</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="14">
         <f t="shared" si="5"/>
         <v>0.70643120843535379</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="O9">
+        <f t="shared" si="6"/>
+        <v>-0.15093012291877395</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10">
         <v>438</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10">
         <v>3.8</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10">
         <v>37264</v>
       </c>
       <c r="F10">
         <v>3.8</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <f t="shared" si="0"/>
         <v>11400000</v>
       </c>
@@ -3191,15 +4360,15 @@
       <c r="I10">
         <v>37264</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="10">
         <f t="shared" si="1"/>
         <v>26027.397260273974</v>
       </c>
-      <c r="K10" s="12" t="str">
+      <c r="K10" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <f t="shared" si="3"/>
         <v>11400000</v>
       </c>
@@ -3207,31 +4376,42 @@
         <f t="shared" si="4"/>
         <v>16321632</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="14">
         <f t="shared" si="5"/>
         <v>0.69845956580812507</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>-0.15585873035823242</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="7"/>
+        <v>0.25</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11">
         <v>260</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11">
         <v>1.73</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11">
         <v>37264</v>
       </c>
       <c r="F11">
         <v>1.73</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <f t="shared" si="0"/>
         <v>5190000</v>
       </c>
@@ -3241,15 +4421,15 @@
       <c r="I11">
         <v>37264</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <f t="shared" si="1"/>
         <v>19961.538461538461</v>
       </c>
-      <c r="K11" s="12" t="str">
+      <c r="K11" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <f t="shared" si="3"/>
         <v>5190000</v>
       </c>
@@ -3257,31 +4437,42 @@
         <f t="shared" si="4"/>
         <v>9688640</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="14">
         <f t="shared" si="5"/>
         <v>0.53567889817353109</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>-0.27109546131296558</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12">
         <v>287</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12">
         <v>3.18</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12">
         <v>37264</v>
       </c>
       <c r="F12">
         <v>3.18</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <f t="shared" si="0"/>
         <v>9540000</v>
       </c>
@@ -3291,15 +4482,15 @@
       <c r="I12">
         <v>37264</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="10">
         <f t="shared" si="1"/>
         <v>33240.4181184669</v>
       </c>
-      <c r="K12" s="12" t="str">
+      <c r="K12" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="10">
         <f t="shared" si="3"/>
         <v>9540000</v>
       </c>
@@ -3307,31 +4498,42 @@
         <f t="shared" si="4"/>
         <v>10694768</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="14">
         <f t="shared" si="5"/>
         <v>0.89202496024224176</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>-4.9622993220502717E-2</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="7"/>
+        <v>0.75</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13">
         <v>245</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13">
         <v>4.18</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13">
         <v>37264</v>
       </c>
       <c r="F13">
         <v>4.18</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <f t="shared" si="0"/>
         <v>12540000</v>
       </c>
@@ -3341,15 +4543,15 @@
       <c r="I13">
         <v>37264</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="10">
         <f t="shared" si="1"/>
         <v>51183.673469387752</v>
       </c>
-      <c r="K13" s="12" t="str">
+      <c r="K13" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="10">
         <f t="shared" si="3"/>
         <v>12540000</v>
       </c>
@@ -3357,31 +4559,42 @@
         <f t="shared" si="4"/>
         <v>9129680</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="14">
         <f t="shared" si="5"/>
         <v>1.3735421175769578</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="O13">
+        <f t="shared" si="6"/>
+        <v>0.13784198093955968</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14">
         <v>75</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14">
         <v>6.12</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14">
         <v>23270</v>
       </c>
       <c r="F14">
         <v>6.12</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="10">
         <f t="shared" si="0"/>
         <v>18360000</v>
       </c>
@@ -3391,15 +4604,15 @@
       <c r="I14">
         <v>23270</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="10">
         <f t="shared" si="1"/>
         <v>244800</v>
       </c>
-      <c r="K14" s="12" t="str">
+      <c r="K14" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Y</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="10">
         <f t="shared" si="3"/>
         <v>4500000</v>
       </c>
@@ -3407,31 +4620,42 @@
         <f t="shared" si="4"/>
         <v>1745250</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="14">
         <f t="shared" si="5"/>
         <v>10.519982810485605</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="O14">
+        <f t="shared" si="6"/>
+        <v>1.0220150301867936</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="7"/>
+        <v>1.25</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15">
         <v>1137</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15">
         <v>6.2</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15">
         <v>13500</v>
       </c>
       <c r="F15">
         <v>6.2</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="10">
         <f t="shared" si="0"/>
         <v>18600000</v>
       </c>
@@ -3441,15 +4665,15 @@
       <c r="I15">
         <v>13500</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="10">
         <f t="shared" si="1"/>
         <v>16358.839050131926</v>
       </c>
-      <c r="K15" s="12" t="str">
+      <c r="K15" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="10">
         <f t="shared" si="3"/>
         <v>18600000</v>
       </c>
@@ -3457,31 +4681,42 @@
         <f t="shared" si="4"/>
         <v>15349500</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="14">
         <f t="shared" si="5"/>
         <v>1.2117658555653279</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="O15">
+        <f t="shared" si="6"/>
+        <v>8.3418711035175425E-2</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16">
         <v>179</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16">
         <v>4.12</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16">
         <v>28176</v>
       </c>
       <c r="F16">
         <v>4.12</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="10">
         <f t="shared" si="0"/>
         <v>12360000</v>
       </c>
@@ -3491,15 +4726,15 @@
       <c r="I16">
         <v>28176</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="10">
         <f t="shared" si="1"/>
         <v>69050.279329608937</v>
       </c>
-      <c r="K16" s="12" t="str">
+      <c r="K16" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Y</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="10">
         <f t="shared" si="3"/>
         <v>10740000</v>
       </c>
@@ -3507,31 +4742,35 @@
         <f t="shared" si="4"/>
         <v>5043504</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="14">
         <f t="shared" si="5"/>
         <v>2.4506771482683467</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="O16">
+        <f t="shared" si="6"/>
+        <v>0.38928610114970214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17">
         <v>17</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17">
         <v>1137</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17">
         <v>60.889999999999993</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17">
         <v>37264</v>
       </c>
       <c r="F17">
         <v>60.889999999999993</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="10">
         <f t="shared" si="0"/>
         <v>182669999.99999997</v>
       </c>
@@ -3542,15 +4781,15 @@
       <c r="I17">
         <v>37264</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="10">
         <f t="shared" si="1"/>
         <v>41421.768707482988</v>
       </c>
-      <c r="K17" s="12" t="str">
+      <c r="K17" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="10">
         <f>SUM(L4:L16)</f>
         <v>119130000</v>
       </c>
@@ -3558,19 +4797,24 @@
         <f>SUM(M4:M16)</f>
         <v>99523220</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="14">
         <f t="shared" si="5"/>
         <v>1.8354510635809409</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L19" s="20">
+      <c r="O17">
+        <f t="shared" si="6"/>
+        <v>0.26374280992413629</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L19" s="19">
         <f>(G17-L17)/G17</f>
         <v>0.34784036787649852</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3592,13 +4836,13 @@
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="18" style="11" customWidth="1"/>
+    <col min="10" max="10" width="18" style="10" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
@@ -3606,7 +4850,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B3" t="s">
@@ -3633,13 +4877,13 @@
       <c r="I3" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="13" t="s">
         <v>80</v>
       </c>
       <c r="M3" t="s">
@@ -3650,25 +4894,25 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4">
         <v>213</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4">
         <v>0.5</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4">
         <v>3338</v>
       </c>
       <c r="F4">
         <v>0.5</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <f>3000000*F4</f>
         <v>1500000</v>
       </c>
@@ -3678,15 +4922,15 @@
       <c r="I4">
         <v>3338</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="10">
         <f>G4/H4</f>
         <v>7042.2535211267605</v>
       </c>
-      <c r="K4" s="12" t="str">
+      <c r="K4" s="11" t="str">
         <f>IF(J4&gt;60000,"Y","")</f>
         <v/>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <f>IF(K4="Y",60000*H4,G4)</f>
         <v>1500000</v>
       </c>
@@ -3694,31 +4938,31 @@
         <f>H4*I4</f>
         <v>710994</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="14">
         <f>G4/M4</f>
         <v>2.109722444915147</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5">
         <v>190</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5">
         <v>6.3000000000000007</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5">
         <v>3338</v>
       </c>
       <c r="F5">
         <v>6.3000000000000007</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <f t="shared" ref="G5:G17" si="0">3000000*F5</f>
         <v>18900000.000000004</v>
       </c>
@@ -3728,15 +4972,15 @@
       <c r="I5">
         <v>3338</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="10">
         <f t="shared" ref="J5:J17" si="1">G5/H5</f>
         <v>99473.684210526335</v>
       </c>
-      <c r="K5" s="12" t="str">
+      <c r="K5" s="11" t="str">
         <f t="shared" ref="K5:K17" si="2">IF(J5&gt;60000,"Y","")</f>
         <v>Y</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <f t="shared" ref="L5:L16" si="3">IF(K5="Y",60000*H5,G5)</f>
         <v>11400000</v>
       </c>
@@ -3744,31 +4988,31 @@
         <f t="shared" ref="M5:M16" si="4">H5*I5</f>
         <v>634220</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="14">
         <f t="shared" ref="N5:N17" si="5">G5/M5</f>
         <v>29.800384724543541</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6">
         <v>78</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6">
         <v>7</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6">
         <v>13132</v>
       </c>
       <c r="F6">
         <v>7</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f t="shared" si="0"/>
         <v>21000000</v>
       </c>
@@ -3778,15 +5022,15 @@
       <c r="I6">
         <v>13132</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <f t="shared" si="1"/>
         <v>269230.76923076925</v>
       </c>
-      <c r="K6" s="12" t="str">
+      <c r="K6" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Y</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <f t="shared" si="3"/>
         <v>4680000</v>
       </c>
@@ -3794,31 +5038,31 @@
         <f t="shared" si="4"/>
         <v>1024296</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="14">
         <f t="shared" si="5"/>
         <v>20.501886173527964</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7">
         <v>261</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7">
         <v>2.04</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>20222</v>
       </c>
       <c r="F7">
         <v>2.04</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <f t="shared" si="0"/>
         <v>6120000</v>
       </c>
@@ -3828,15 +5072,15 @@
       <c r="I7">
         <v>20222</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <f t="shared" si="1"/>
         <v>23448.275862068964</v>
       </c>
-      <c r="K7" s="12" t="str">
+      <c r="K7" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <f t="shared" si="3"/>
         <v>6120000</v>
       </c>
@@ -3844,31 +5088,31 @@
         <f t="shared" si="4"/>
         <v>5277942</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="14">
         <f t="shared" si="5"/>
         <v>1.1595428672766772</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8">
         <v>132</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8">
         <v>10.719999999999999</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8">
         <v>20222</v>
       </c>
       <c r="F8">
         <v>10.719999999999999</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <f t="shared" si="0"/>
         <v>32159999.999999996</v>
       </c>
@@ -3878,15 +5122,15 @@
       <c r="I8">
         <v>20222</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <f t="shared" si="1"/>
         <v>243636.36363636362</v>
       </c>
-      <c r="K8" s="12" t="str">
+      <c r="K8" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Y</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <f t="shared" si="3"/>
         <v>7920000</v>
       </c>
@@ -3894,31 +5138,31 @@
         <f t="shared" si="4"/>
         <v>2669304</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="14">
         <f t="shared" si="5"/>
         <v>12.048084444484404</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>915</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9">
         <v>5</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>23206</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <f t="shared" si="0"/>
         <v>15000000</v>
       </c>
@@ -3928,15 +5172,15 @@
       <c r="I9">
         <v>23206</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <f t="shared" si="1"/>
         <v>16393.442622950821</v>
       </c>
-      <c r="K9" s="12" t="str">
+      <c r="K9" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <f t="shared" si="3"/>
         <v>15000000</v>
       </c>
@@ -3944,31 +5188,31 @@
         <f t="shared" si="4"/>
         <v>21233490</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="14">
         <f t="shared" si="5"/>
         <v>0.70643120843535379</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10">
         <v>438</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10">
         <v>3.8</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10">
         <v>37264</v>
       </c>
       <c r="F10">
         <v>3.8</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <f t="shared" si="0"/>
         <v>11400000</v>
       </c>
@@ -3978,15 +5222,15 @@
       <c r="I10">
         <v>37264</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="10">
         <f t="shared" si="1"/>
         <v>26027.397260273974</v>
       </c>
-      <c r="K10" s="12" t="str">
+      <c r="K10" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <f t="shared" si="3"/>
         <v>11400000</v>
       </c>
@@ -3994,31 +5238,31 @@
         <f t="shared" si="4"/>
         <v>16321632</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="14">
         <f t="shared" si="5"/>
         <v>0.69845956580812507</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11">
         <v>260</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11">
         <v>1.73</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11">
         <v>37264</v>
       </c>
       <c r="F11">
         <v>1.73</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <f t="shared" si="0"/>
         <v>5190000</v>
       </c>
@@ -4028,15 +5272,15 @@
       <c r="I11">
         <v>37264</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <f t="shared" si="1"/>
         <v>19961.538461538461</v>
       </c>
-      <c r="K11" s="12" t="str">
+      <c r="K11" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <f t="shared" si="3"/>
         <v>5190000</v>
       </c>
@@ -4044,31 +5288,31 @@
         <f t="shared" si="4"/>
         <v>9688640</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="14">
         <f t="shared" si="5"/>
         <v>0.53567889817353109</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12">
         <v>287</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12">
         <v>3.18</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12">
         <v>37264</v>
       </c>
       <c r="F12">
         <v>3.18</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <f t="shared" si="0"/>
         <v>9540000</v>
       </c>
@@ -4078,15 +5322,15 @@
       <c r="I12">
         <v>37264</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="10">
         <f t="shared" si="1"/>
         <v>33240.4181184669</v>
       </c>
-      <c r="K12" s="12" t="str">
+      <c r="K12" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="10">
         <f t="shared" si="3"/>
         <v>9540000</v>
       </c>
@@ -4094,31 +5338,31 @@
         <f t="shared" si="4"/>
         <v>10694768</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="14">
         <f t="shared" si="5"/>
         <v>0.89202496024224176</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13">
         <v>245</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13">
         <v>4.18</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13">
         <v>37264</v>
       </c>
       <c r="F13">
         <v>4.18</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <f t="shared" si="0"/>
         <v>12540000</v>
       </c>
@@ -4128,15 +5372,15 @@
       <c r="I13">
         <v>37264</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="10">
         <f t="shared" si="1"/>
         <v>51183.673469387752</v>
       </c>
-      <c r="K13" s="12" t="str">
+      <c r="K13" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="10">
         <f t="shared" si="3"/>
         <v>12540000</v>
       </c>
@@ -4144,31 +5388,31 @@
         <f t="shared" si="4"/>
         <v>9129680</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="14">
         <f t="shared" si="5"/>
         <v>1.3735421175769578</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14">
         <v>75</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14">
         <v>6.12</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14">
         <v>23270</v>
       </c>
       <c r="F14">
         <v>6.12</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="10">
         <f t="shared" si="0"/>
         <v>18360000</v>
       </c>
@@ -4178,15 +5422,15 @@
       <c r="I14">
         <v>23270</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="10">
         <f t="shared" si="1"/>
         <v>244800</v>
       </c>
-      <c r="K14" s="12" t="str">
+      <c r="K14" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Y</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="10">
         <f t="shared" si="3"/>
         <v>4500000</v>
       </c>
@@ -4194,31 +5438,31 @@
         <f t="shared" si="4"/>
         <v>1745250</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="14">
         <f t="shared" si="5"/>
         <v>10.519982810485605</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15">
         <v>1137</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15">
         <v>6.2</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15">
         <v>13500</v>
       </c>
       <c r="F15">
         <v>6.2</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="10">
         <f t="shared" si="0"/>
         <v>18600000</v>
       </c>
@@ -4228,15 +5472,15 @@
       <c r="I15">
         <v>13500</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="10">
         <f t="shared" si="1"/>
         <v>16358.839050131926</v>
       </c>
-      <c r="K15" s="12" t="str">
+      <c r="K15" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="10">
         <f t="shared" si="3"/>
         <v>18600000</v>
       </c>
@@ -4244,31 +5488,31 @@
         <f t="shared" si="4"/>
         <v>15349500</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="14">
         <f t="shared" si="5"/>
         <v>1.2117658555653279</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16">
         <v>179</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16">
         <v>4.12</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16">
         <v>28176</v>
       </c>
       <c r="F16">
         <v>4.12</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="10">
         <f t="shared" si="0"/>
         <v>12360000</v>
       </c>
@@ -4278,15 +5522,15 @@
       <c r="I16">
         <v>28176</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="10">
         <f t="shared" si="1"/>
         <v>69050.279329608937</v>
       </c>
-      <c r="K16" s="12" t="str">
+      <c r="K16" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Y</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="10">
         <f t="shared" si="3"/>
         <v>10740000</v>
       </c>
@@ -4294,31 +5538,31 @@
         <f t="shared" si="4"/>
         <v>5043504</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="14">
         <f t="shared" si="5"/>
         <v>2.4506771482683467</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17">
         <v>17</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17">
         <v>1137</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17">
         <v>60.889999999999993</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17">
         <v>37264</v>
       </c>
       <c r="F17">
         <v>60.889999999999993</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="10">
         <f t="shared" si="0"/>
         <v>182669999.99999997</v>
       </c>
@@ -4329,15 +5573,15 @@
       <c r="I17">
         <v>37264</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="10">
         <f t="shared" si="1"/>
         <v>41421.768707482988</v>
       </c>
-      <c r="K17" s="12" t="str">
+      <c r="K17" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="10">
         <f>SUM(L4:L16)</f>
         <v>119130000</v>
       </c>
@@ -4345,7 +5589,7 @@
         <f>SUM(M4:M16)</f>
         <v>99523220</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="14">
         <f t="shared" si="5"/>
         <v>1.8354510635809409</v>
       </c>
@@ -4356,6 +5600,156 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <QuestionsinDR xmlns="2104ad18-0c40-4759-978d-9031b6355d10" xsi:nil="true"/>
+    <Comment xmlns="2104ad18-0c40-4759-978d-9031b6355d10" xsi:nil="true"/>
+    <SharedWithUsers xmlns="80a17f64-e774-4a01-b2f5-de7df872f7b3">
+      <UserInfo>
+        <DisplayName>Gahagan, Shaun</DisplayName>
+        <AccountId>390</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kloberdanz, Kari</DisplayName>
+        <AccountId>3271</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Valencia, Isaiah (Contractor)</DisplayName>
+        <AccountId>3488</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Mauer, Katie</DisplayName>
+        <AccountId>55</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Nimick, Jan A (Contractor)</DisplayName>
+        <AccountId>4096</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>McMillin, Lena</DisplayName>
+        <AccountId>86</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas, Willie</DisplayName>
+        <AccountId>42</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Gabriel, Robert</DisplayName>
+        <AccountId>1819</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Estrada, Juan</DisplayName>
+        <AccountId>2607</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Smith, Caitlin G</DisplayName>
+        <AccountId>2742</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Parikh, Minal K</DisplayName>
+        <AccountId>178</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Fallon, Cassandra A</DisplayName>
+        <AccountId>2983</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Knowd, Tim M.</DisplayName>
+        <AccountId>169</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Woldemariam, Jonathan</DisplayName>
+        <AccountId>32</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>DeLouis, Bobby</DisplayName>
+        <AccountId>3555</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Menon, Nisha</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Taylor, Cynthia S</DisplayName>
+        <AccountId>702</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Woldegiorgis, Shewit T</DisplayName>
+        <AccountId>940</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Davis, Erick (Contractor)</DisplayName>
+        <AccountId>2156</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Fulton, Laura M</DisplayName>
+        <AccountId>689</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Makhamreh, Mazen (Contractor)</DisplayName>
+        <AccountId>30</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sebastian Peral, Joaquin</DisplayName>
+        <AccountId>46</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Black, John (Contractor)</DisplayName>
+        <AccountId>4098</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Flamenbaum, Robert</DisplayName>
+        <AccountId>45</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Bertolini, Crystal A</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Cui, Landy Ye</DisplayName>
+        <AccountId>162</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Biscay, Cameron H</DisplayName>
+        <AccountId>4152</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2104ad18-0c40-4759-978d-9031b6355d10">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="80a17f64-e774-4a01-b2f5-de7df872f7b3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007BC5B34FB2B05C498322EC0E0E7F8BBD" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c243bf6f29386086e21656a0b091e581">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2104ad18-0c40-4759-978d-9031b6355d10" xmlns:ns3="80a17f64-e774-4a01-b2f5-de7df872f7b3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4bbf6d1ef2da01010e564fac80a0ca5f" ns2:_="" ns3:_="">
     <xsd:import namespace="2104ad18-0c40-4759-978d-9031b6355d10"/>
@@ -4620,7 +6014,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4629,157 +6023,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <QuestionsinDR xmlns="2104ad18-0c40-4759-978d-9031b6355d10" xsi:nil="true"/>
-    <Comment xmlns="2104ad18-0c40-4759-978d-9031b6355d10" xsi:nil="true"/>
-    <SharedWithUsers xmlns="80a17f64-e774-4a01-b2f5-de7df872f7b3">
-      <UserInfo>
-        <DisplayName>Gahagan, Shaun</DisplayName>
-        <AccountId>390</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kloberdanz, Kari</DisplayName>
-        <AccountId>3271</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Valencia, Isaiah (Contractor)</DisplayName>
-        <AccountId>3488</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Mauer, Katie</DisplayName>
-        <AccountId>55</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Nimick, Jan A (Contractor)</DisplayName>
-        <AccountId>4096</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>McMillin, Lena</DisplayName>
-        <AccountId>86</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas, Willie</DisplayName>
-        <AccountId>42</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Gabriel, Robert</DisplayName>
-        <AccountId>1819</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Estrada, Juan</DisplayName>
-        <AccountId>2607</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Smith, Caitlin G</DisplayName>
-        <AccountId>2742</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Parikh, Minal K</DisplayName>
-        <AccountId>178</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Fallon, Cassandra A</DisplayName>
-        <AccountId>2983</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Knowd, Tim M.</DisplayName>
-        <AccountId>169</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Woldemariam, Jonathan</DisplayName>
-        <AccountId>32</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>DeLouis, Bobby</DisplayName>
-        <AccountId>3555</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Menon, Nisha</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Taylor, Cynthia S</DisplayName>
-        <AccountId>702</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Woldegiorgis, Shewit T</DisplayName>
-        <AccountId>940</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Davis, Erick (Contractor)</DisplayName>
-        <AccountId>2156</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Fulton, Laura M</DisplayName>
-        <AccountId>689</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Makhamreh, Mazen (Contractor)</DisplayName>
-        <AccountId>30</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sebastian Peral, Joaquin</DisplayName>
-        <AccountId>46</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Black, John (Contractor)</DisplayName>
-        <AccountId>4098</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Flamenbaum, Robert</DisplayName>
-        <AccountId>45</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Bertolini, Crystal A</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Cui, Landy Ye</DisplayName>
-        <AccountId>162</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Biscay, Cameron H</DisplayName>
-        <AccountId>4152</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2104ad18-0c40-4759-978d-9031b6355d10">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="80a17f64-e774-4a01-b2f5-de7df872f7b3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{626DCC1C-599C-4BE6-905F-8E05ADF5ABE4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="80a17f64-e774-4a01-b2f5-de7df872f7b3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2104ad18-0c40-4759-978d-9031b6355d10"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CD48C82-D666-4629-85AF-3D6475D67B63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4798,27 +6059,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4422F3FD-98DC-4FAA-8797-19A7CD709955}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{626DCC1C-599C-4BE6-905F-8E05ADF5ABE4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="80a17f64-e774-4a01-b2f5-de7df872f7b3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2104ad18-0c40-4759-978d-9031b6355d10"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>